<commit_message>
improvement backend & ui
</commit_message>
<xml_diff>
--- a/backend/node/data/demo.xlsx
+++ b/backend/node/data/demo.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -430,9 +430,23 @@
         <v>user</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>asu@gmail.com</v>
+      </c>
+      <c r="B3" t="str">
+        <v>ed9c139d8f537c8b631ccc0258c9b570a9fdf723329871a1560c90ba0c95d439</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="str">
+        <v>user</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>